<commit_message>
Logica de Mesas 01/03
</commit_message>
<xml_diff>
--- a/Menu.xlsx
+++ b/Menu.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jluis\Documents\NetBeansProjects\Angels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A99586C-1B41-4557-8534-B8211C4C1D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA263705-C074-41DB-9A62-7D88FE04728D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{EDE3319B-5F1A-4311-8C62-2FA953424D04}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{EDE3319B-5F1A-4311-8C62-2FA953424D04}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,9 +267,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{219DC8AF-527D-46D6-81A0-87CD3EE8CAA8}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J69" sqref="J69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +619,7 @@
       <c r="B4">
         <v>75</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
     </row>
@@ -609,6 +630,7 @@
       <c r="B5">
         <v>60</v>
       </c>
+      <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -617,6 +639,7 @@
       <c r="B6">
         <v>60</v>
       </c>
+      <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -625,6 +648,7 @@
       <c r="B7">
         <v>50</v>
       </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -633,11 +657,13 @@
       <c r="B8">
         <v>50</v>
       </c>
+      <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -646,6 +672,7 @@
       <c r="B10">
         <v>15</v>
       </c>
+      <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -654,6 +681,7 @@
       <c r="B11">
         <v>20</v>
       </c>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -662,6 +690,7 @@
       <c r="B12">
         <v>15</v>
       </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -670,6 +699,7 @@
       <c r="B13">
         <v>20</v>
       </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -678,6 +708,7 @@
       <c r="B14">
         <v>20</v>
       </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -686,6 +717,7 @@
       <c r="B15">
         <v>20</v>
       </c>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -694,354 +726,398 @@
       <c r="B16">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17">
         <v>30</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24">
         <v>50</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25">
         <v>50</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
       <c r="B27">
         <v>15</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
       <c r="B28">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
       <c r="B29">
         <v>40</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
       <c r="B30">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>26</v>
       </c>
       <c r="B31">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>27</v>
       </c>
       <c r="B32">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>33</v>
       </c>
       <c r="B34">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>34</v>
       </c>
       <c r="B35">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
       <c r="B37">
         <v>50</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>38</v>
       </c>
       <c r="B39">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" s="4"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>39</v>
       </c>
       <c r="B40">
         <v>50</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>40</v>
       </c>
       <c r="B41">
         <v>75</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>41</v>
       </c>
       <c r="B42">
         <v>40</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
       <c r="B43">
         <v>75</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
       <c r="B44">
         <v>125</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>44</v>
       </c>
       <c r="B45">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
       <c r="B46">
         <v>75</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" s="4"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>46</v>
       </c>
       <c r="B47">
         <v>125</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" s="4"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
       <c r="B49">
         <v>75</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" s="4"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
       <c r="B51">
         <v>60</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>51</v>
       </c>
       <c r="B52">
         <v>60</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>52</v>
       </c>
       <c r="B53">
         <v>60</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>53</v>
       </c>
       <c r="B54">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>54</v>
       </c>
       <c r="B55">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>55</v>
       </c>
       <c r="B56">
         <v>160</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" s="4"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>56</v>
       </c>
       <c r="B57">
         <v>60</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>57</v>
       </c>
       <c r="B58">
         <v>60</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>58</v>
       </c>
       <c r="B59">
         <v>85</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>59</v>
       </c>
       <c r="B60">
         <v>35</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" s="4"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>60</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
+      <c r="C61" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>